<commit_message>
Fixed the diagonal values in diagM
</commit_message>
<xml_diff>
--- a/data/Wd.xlsx
+++ b/data/Wd.xlsx
@@ -404,7 +404,7 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2">
-        <v>159.94000000000003</v>
+        <v>14.540000000000001</v>
       </c>
       <c r="B2">
         <v>0.0</v>
@@ -418,7 +418,7 @@
         <v>0.0</v>
       </c>
       <c r="B3">
-        <v>0.15400000000000003</v>
+        <v>0.014000000000000002</v>
       </c>
       <c r="C3">
         <v>0.0</v>
@@ -432,7 +432,7 @@
         <v>0.0</v>
       </c>
       <c r="C4">
-        <v>3.6817</v>
+        <v>0.3347</v>
       </c>
     </row>
   </sheetData>

</xml_diff>